<commit_message>
Implementation de la fenetre Phylogeny
</commit_message>
<xml_diff>
--- a/other_files/phylogeny.xlsx
+++ b/other_files/phylogeny.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Coraux" sheetId="1" r:id="rId1"/>
+    <sheet name="Herbiers" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="154">
   <si>
     <t>Acroporidae</t>
   </si>
@@ -474,6 +475,18 @@
   </si>
   <si>
     <t>Arachnactidae</t>
+  </si>
+  <si>
+    <t>Classe</t>
+  </si>
+  <si>
+    <t>Sous-classe</t>
+  </si>
+  <si>
+    <t>Ordre</t>
+  </si>
+  <si>
+    <t>Famille</t>
   </si>
 </sst>
 </file>
@@ -810,10 +823,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D150"/>
+  <dimension ref="A1:D151"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -825,758 +838,784 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D4" s="1" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D5" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D6" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D7" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D8" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D9" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D10" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D11" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D12" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D13" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D14" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D15" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D16" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D17" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D17" s="1" t="s">
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D18" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D18" s="1" t="s">
+    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D19" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D19" s="1" t="s">
+    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D20" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D20" s="1" t="s">
+    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D21" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D21" s="1" t="s">
+    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D22" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D22" s="1" t="s">
+    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D23" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D23" s="1" t="s">
+    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D24" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D24" s="1" t="s">
+    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D25" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D25" s="1" t="s">
+    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D26" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D26" s="1" t="s">
+    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D27" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D27" s="1" t="s">
+    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D28" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D28" s="1" t="s">
+    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D29" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D29" s="1" t="s">
+    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D30" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D30" s="1" t="s">
+    <row r="31" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D31" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D31" s="1" t="s">
+    <row r="32" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D32" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C32" t="s">
+    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D33" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="34" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="35" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D35" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C36" t="s">
+    <row r="37" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="37" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D37" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="38" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D38" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="39" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="41" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="42" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D42" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D43" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C43" t="s">
+    <row r="44" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="44" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D44" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="45" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D45" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="46" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D46" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="47" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D47" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="48" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D49" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D50" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D51" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D52" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D53" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C54" t="s">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D55" s="1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D56" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D57" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D58" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D59" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D60" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D61" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D62" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D63" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D64" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="65" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D65" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="66" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D66" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="67" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D67" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="68" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D68" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="69" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D69" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="70" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D70" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D70" s="2" t="s">
+    <row r="71" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D71" s="2" t="s">
         <v>69</v>
-      </c>
-    </row>
-    <row r="71" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D71" s="1" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="72" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D72" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="73" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D73" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="74" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D74" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="75" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D75" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="76" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D76" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="77" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D77" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="78" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D78" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D78" s="3" t="s">
+    <row r="79" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D79" s="3" t="s">
         <v>77</v>
-      </c>
-    </row>
-    <row r="79" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D79" s="1" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="80" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D80" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="81" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D81" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D81" s="1" t="s">
+    <row r="82" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D82" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D82" s="1" t="s">
+    <row r="83" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D83" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="83" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D83" s="1" t="s">
+    <row r="84" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D84" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="84" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D84" s="1" t="s">
+    <row r="85" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D85" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="85" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D85" s="1" t="s">
+    <row r="86" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D86" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="86" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D86" s="1" t="s">
+    <row r="87" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D87" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="87" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D87" s="1" t="s">
+    <row r="88" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D88" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="88" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D88" s="1" t="s">
+    <row r="89" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D89" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="89" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D89" s="1" t="s">
+    <row r="90" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D90" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="90" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D90" s="1" t="s">
+    <row r="91" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D91" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="91" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D91" s="1" t="s">
+    <row r="92" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D92" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="92" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D92" s="1" t="s">
+    <row r="93" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D93" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="93" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D93" s="1" t="s">
+    <row r="94" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D94" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="94" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D94" s="1" t="s">
+    <row r="95" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D95" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="95" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D95" s="1" t="s">
+    <row r="96" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D96" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="96" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C96" t="s">
+    <row r="97" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C97" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="97" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D97" s="1" t="s">
+    <row r="98" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D98" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="98" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D98" s="1" t="s">
+    <row r="99" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D99" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="99" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D99" s="1" t="s">
+    <row r="100" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D100" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="100" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D100" s="1" t="s">
+    <row r="101" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D101" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="101" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D101" s="1" t="s">
+    <row r="102" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D102" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="102" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D102" s="1" t="s">
+    <row r="103" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D103" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="103" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D103" s="1" t="s">
+    <row r="104" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D104" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="104" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D104" s="1" t="s">
+    <row r="105" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D105" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="105" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D105" s="1" t="s">
+    <row r="106" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D106" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="106" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D106" s="1" t="s">
+    <row r="107" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D107" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="107" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D107" s="1" t="s">
+    <row r="108" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D108" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="108" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D108" s="1" t="s">
+    <row r="109" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D109" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="109" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D109" s="1" t="s">
+    <row r="110" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D110" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="110" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D110" s="1" t="s">
+    <row r="111" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D111" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="111" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D111" s="1" t="s">
+    <row r="112" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D112" s="1" t="s">
         <v>110</v>
-      </c>
-    </row>
-    <row r="112" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D112" s="1" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="113" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D113" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="114" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D114" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="115" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D115" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="116" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D116" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="117" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D117" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="118" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D118" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="119" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D119" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="120" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D120" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="121" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D121" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="122" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D122" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="123" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D123" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="124" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D124" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="125" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D125" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="126" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D126" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="127" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D127" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="128" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D128" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="129" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D129" s="1" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="129" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C129" t="s">
+    <row r="130" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C130" t="s">
         <v>128</v>
-      </c>
-    </row>
-    <row r="130" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D130" s="1" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="131" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D131" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="132" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D132" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="133" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D133" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="134" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D134" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="135" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D135" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="136" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D136" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="137" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D137" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="138" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D138" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="139" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D139" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="140" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D140" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="141" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D141" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="142" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D142" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="143" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D143" s="1" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="143" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C143" t="s">
+    <row r="144" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C144" t="s">
         <v>142</v>
-      </c>
-    </row>
-    <row r="144" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D144" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="145" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D145" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="146" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D146" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="146" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B146" t="s">
+    <row r="147" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B147" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="147" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C147" t="s">
+    <row r="148" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C148" t="s">
         <v>146</v>
-      </c>
-    </row>
-    <row r="148" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D148" s="1" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="149" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D149" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="150" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D150" s="1" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="150" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D150" t="s">
+    <row r="151" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D151" t="s">
         <v>149</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D78" r:id="rId1" tooltip="family" display="https://www.ncbi.nlm.nih.gov/Taxonomy/Browser/wwwtax.cgi?mode=Tree&amp;id=478439&amp;lvl=3&amp;lin=f&amp;keep=1&amp;srchmode=1&amp;unlock"/>
+    <hyperlink ref="D79" r:id="rId1" tooltip="family" display="https://www.ncbi.nlm.nih.gov/Taxonomy/Browser/wwwtax.cgi?mode=Tree&amp;id=478439&amp;lvl=3&amp;lin=f&amp;keep=1&amp;srchmode=1&amp;unlock"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Implementation de la taxonomie générale des herbiers
</commit_message>
<xml_diff>
--- a/other_files/phylogeny.xlsx
+++ b/other_files/phylogeny.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="171">
   <si>
     <t>Acroporidae</t>
   </si>
@@ -487,6 +487,57 @@
   </si>
   <si>
     <t>Famille</t>
+  </si>
+  <si>
+    <t>Genre</t>
+  </si>
+  <si>
+    <t>Zosteraceae</t>
+  </si>
+  <si>
+    <t>Heterozostera</t>
+  </si>
+  <si>
+    <t>Phyllospadix</t>
+  </si>
+  <si>
+    <t>Zostera</t>
+  </si>
+  <si>
+    <t>Posidoniaceae</t>
+  </si>
+  <si>
+    <t>Posidonia</t>
+  </si>
+  <si>
+    <t>Cymodoceaceae</t>
+  </si>
+  <si>
+    <t>Amphibolis</t>
+  </si>
+  <si>
+    <t>Cymodocea</t>
+  </si>
+  <si>
+    <t>Halodule</t>
+  </si>
+  <si>
+    <t>Syringodium</t>
+  </si>
+  <si>
+    <t>Thalassodendron</t>
+  </si>
+  <si>
+    <t>Hydrocharitaceae</t>
+  </si>
+  <si>
+    <t>Enhalus</t>
+  </si>
+  <si>
+    <t>Halophila</t>
+  </si>
+  <si>
+    <t>Thalassia</t>
   </si>
 </sst>
 </file>
@@ -826,7 +877,7 @@
   <dimension ref="A1:D151"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1610,12 +1661,107 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>170</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ajout de la phylogenie des paletuviers
</commit_message>
<xml_diff>
--- a/other_files/phylogeny.xlsx
+++ b/other_files/phylogeny.xlsx
@@ -13,7 +13,8 @@
   </bookViews>
   <sheets>
     <sheet name="Coraux" sheetId="1" r:id="rId1"/>
-    <sheet name="Herbiers" sheetId="2" r:id="rId2"/>
+    <sheet name="Mangroves" sheetId="3" r:id="rId2"/>
+    <sheet name="Herbiers" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="200">
   <si>
     <t>Acroporidae</t>
   </si>
@@ -538,6 +539,93 @@
   </si>
   <si>
     <t>Thalassia</t>
+  </si>
+  <si>
+    <t>Embranchement</t>
+  </si>
+  <si>
+    <t>Tracheophyta</t>
+  </si>
+  <si>
+    <t>Magnoliopsida</t>
+  </si>
+  <si>
+    <t>Lamiales</t>
+  </si>
+  <si>
+    <t>Avicenniaceae</t>
+  </si>
+  <si>
+    <t>Acanthus ebracteatus</t>
+  </si>
+  <si>
+    <t>Avicennia marina</t>
+  </si>
+  <si>
+    <t>Avicennia officinalis</t>
+  </si>
+  <si>
+    <t>Myrtales</t>
+  </si>
+  <si>
+    <t>Lythraceae</t>
+  </si>
+  <si>
+    <t>Sonneratia alba</t>
+  </si>
+  <si>
+    <t>Primulales</t>
+  </si>
+  <si>
+    <t>Myrsinaceae</t>
+  </si>
+  <si>
+    <t>Aegiceras corniculatum</t>
+  </si>
+  <si>
+    <t>Rhizophorales</t>
+  </si>
+  <si>
+    <t>Rhizophoraceae</t>
+  </si>
+  <si>
+    <t>Bruguiera gymnorhiza</t>
+  </si>
+  <si>
+    <t>Bruguiera sexangula</t>
+  </si>
+  <si>
+    <t>Kandelia candel</t>
+  </si>
+  <si>
+    <t>Kandelia obovata</t>
+  </si>
+  <si>
+    <t>Rhizophora apiculata</t>
+  </si>
+  <si>
+    <t>Rhizophora mangle</t>
+  </si>
+  <si>
+    <t>Rhizophora stylosa</t>
+  </si>
+  <si>
+    <t>Monocotyledoneae</t>
+  </si>
+  <si>
+    <t>Arecales</t>
+  </si>
+  <si>
+    <t>Arecaceae</t>
+  </si>
+  <si>
+    <t>Nypa fruticans</t>
+  </si>
+  <si>
+    <t>Phoenix paludosa</t>
+  </si>
+  <si>
+    <t>Espece</t>
   </si>
 </sst>
 </file>
@@ -588,11 +676,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -1661,9 +1751,183 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="E1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="4" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C4" s="4" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D5" s="5" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E7" s="4" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D10" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D13" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D16" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D26" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E28" t="s">
+        <v>198</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Debug du telechargement de produit + petit changement + ajout donnees mangrove
</commit_message>
<xml_diff>
--- a/other_files/phylogeny.xlsx
+++ b/other_files/phylogeny.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="198">
   <si>
     <t>Acroporidae</t>
   </si>
@@ -556,9 +556,6 @@
     <t>Avicenniaceae</t>
   </si>
   <si>
-    <t>Acanthus ebracteatus</t>
-  </si>
-  <si>
     <t>Avicennia marina</t>
   </si>
   <si>
@@ -620,9 +617,6 @@
   </si>
   <si>
     <t>Nypa fruticans</t>
-  </si>
-  <si>
-    <t>Phoenix paludosa</t>
   </si>
   <si>
     <t>Espece</t>
@@ -1751,10 +1745,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1780,7 +1774,7 @@
         <v>153</v>
       </c>
       <c r="E1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1804,57 +1798,57 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E6" t="s">
+      <c r="E6" s="4" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E7" s="4" t="s">
+      <c r="E7" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E8" t="s">
+      <c r="C8" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
+      <c r="D9" s="1" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D10" s="1" t="s">
+      <c r="E10" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E11" t="s">
+      <c r="C11" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
+      <c r="D12" s="1" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D13" s="1" t="s">
+      <c r="E13" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E14" t="s">
+      <c r="C14" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
+      <c r="D15" s="1" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D16" s="1" t="s">
+      <c r="E16" t="s">
         <v>186</v>
       </c>
     </row>
@@ -1889,33 +1883,23 @@
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E23" t="s">
+      <c r="B23" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C25" t="s">
+      <c r="D25" s="1" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D26" s="1" t="s">
+      <c r="E26" t="s">
         <v>196</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E27" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E28" t="s">
-        <v>198</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajout d'espece de mangrove
</commit_message>
<xml_diff>
--- a/other_files/phylogeny.xlsx
+++ b/other_files/phylogeny.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="245">
   <si>
     <t>Acroporidae</t>
   </si>
@@ -595,31 +595,172 @@
     <t>Kandelia candel</t>
   </si>
   <si>
+    <t>Rhizophora apiculata</t>
+  </si>
+  <si>
+    <t>Rhizophora mangle</t>
+  </si>
+  <si>
+    <t>Rhizophora stylosa</t>
+  </si>
+  <si>
+    <t>Monocotyledoneae</t>
+  </si>
+  <si>
+    <t>Arecales</t>
+  </si>
+  <si>
+    <t>Arecaceae</t>
+  </si>
+  <si>
+    <t>Nypa fruticans</t>
+  </si>
+  <si>
+    <t>Espece</t>
+  </si>
+  <si>
+    <t>Caryophyllales</t>
+  </si>
+  <si>
+    <t>Sapindales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chenopodiaceae </t>
+  </si>
+  <si>
+    <t>Suaeda monoica</t>
+  </si>
+  <si>
+    <t>Plumbaginaceae</t>
+  </si>
+  <si>
+    <t>Aegialitis annulata</t>
+  </si>
+  <si>
+    <t>Aegialitis rotundifolia</t>
+  </si>
+  <si>
+    <t>Avicennia alba</t>
+  </si>
+  <si>
+    <t>Avicennia bicolor</t>
+  </si>
+  <si>
+    <t>Avicennia germinans</t>
+  </si>
+  <si>
+    <t>Avicennia integra</t>
+  </si>
+  <si>
+    <t>Avicennia rumphiana</t>
+  </si>
+  <si>
+    <t>Avicennia schaueriana</t>
+  </si>
+  <si>
+    <t>Avicennia tonduzii</t>
+  </si>
+  <si>
+    <t>Combretaceae</t>
+  </si>
+  <si>
+    <t>Conocarpus erectus</t>
+  </si>
+  <si>
+    <t>Conocarpus lancifolius</t>
+  </si>
+  <si>
+    <t>Conocarpus sericeus</t>
+  </si>
+  <si>
+    <t>Laguncularia racemosa</t>
+  </si>
+  <si>
+    <t>Lumnitzera littorea</t>
+  </si>
+  <si>
+    <t>Lumnitzera racemosa</t>
+  </si>
+  <si>
+    <t>Lumnitzera rosea</t>
+  </si>
+  <si>
+    <t>Sonneratia apetala</t>
+  </si>
+  <si>
+    <t>Sonneratia caseolaris</t>
+  </si>
+  <si>
+    <t>Sonneratia griffithii</t>
+  </si>
+  <si>
+    <t>Sonneratia lanceolata</t>
+  </si>
+  <si>
+    <t>Sonneratia ovata</t>
+  </si>
+  <si>
+    <t>Sonneratia paracaseolaris</t>
+  </si>
+  <si>
+    <t>Aegiceras floridum</t>
+  </si>
+  <si>
+    <t>Bruguiera cylindrica</t>
+  </si>
+  <si>
+    <t>Bruguiera exaristata</t>
+  </si>
+  <si>
+    <t>Bruguiera hainesii</t>
+  </si>
+  <si>
+    <t>Bruguiera parviflora</t>
+  </si>
+  <si>
+    <t>Ceriops australis</t>
+  </si>
+  <si>
+    <t>Ceriops decandra</t>
+  </si>
+  <si>
+    <t>Ceriops pseudodecandra</t>
+  </si>
+  <si>
+    <t>Ceriops tagal</t>
+  </si>
+  <si>
+    <t>Ceriops zippeliana</t>
+  </si>
+  <si>
+    <t>Rhizophora mucronata   </t>
+  </si>
+  <si>
+    <t>Rhizophora racemosa</t>
+  </si>
+  <si>
+    <t>Rhizophora samoensis   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meliaceae </t>
+  </si>
+  <si>
+    <t>Xylocarpus granatum</t>
+  </si>
+  <si>
+    <t>Xylocarpus mekongensis</t>
+  </si>
+  <si>
+    <t>Xylocarpus moluccensis</t>
+  </si>
+  <si>
+    <t>Xylocarpus procerus</t>
+  </si>
+  <si>
+    <t>Xylocarpus rumphii</t>
+  </si>
+  <si>
     <t>Kandelia obovata</t>
-  </si>
-  <si>
-    <t>Rhizophora apiculata</t>
-  </si>
-  <si>
-    <t>Rhizophora mangle</t>
-  </si>
-  <si>
-    <t>Rhizophora stylosa</t>
-  </si>
-  <si>
-    <t>Monocotyledoneae</t>
-  </si>
-  <si>
-    <t>Arecales</t>
-  </si>
-  <si>
-    <t>Arecaceae</t>
-  </si>
-  <si>
-    <t>Nypa fruticans</t>
-  </si>
-  <si>
-    <t>Espece</t>
   </si>
 </sst>
 </file>
@@ -670,13 +811,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -1745,10 +1885,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="E56" sqref="E56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1774,7 +1914,7 @@
         <v>153</v>
       </c>
       <c r="E1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1788,118 +1928,360 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C4" s="4" t="s">
+      <c r="C4" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D7" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C8" s="4"/>
+      <c r="E8" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C9" s="4"/>
+      <c r="E9" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C10" s="4" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D5" s="5" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C11" s="4"/>
+      <c r="D11" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E6" s="4" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E7" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D9" s="1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E10" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
-        <v>181</v>
-      </c>
-    </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D12" s="1" t="s">
-        <v>182</v>
+      <c r="C12" s="4"/>
+      <c r="E12" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C13" s="4"/>
       <c r="E13" t="s">
-        <v>183</v>
+        <v>205</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C14" t="s">
-        <v>184</v>
+      <c r="C14" s="4"/>
+      <c r="E14" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D15" s="1" t="s">
-        <v>185</v>
+      <c r="C15" s="4"/>
+      <c r="E15" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E16" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="21" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="22" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="23" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="24" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="25" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="26" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E26" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="27" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="28" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E28" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="29" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E29" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="30" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D30" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="31" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E31" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="32" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E32" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="33" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E33" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="34" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E34" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="35" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E35" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="36" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E36" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="37" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E37" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="38" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="39" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D39" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="40" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E40" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="41" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E41" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="42" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="43" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D43" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="44" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E44" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="45" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E45" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="46" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E46" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E17" t="s">
+    <row r="47" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E47" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="48" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E48" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="49" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E49" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E18" t="s">
+    <row r="50" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E50" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="51" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E51" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="52" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E52" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="53" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E53" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="54" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E54" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="55" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E55" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E19" t="s">
+    <row r="56" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E56" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="57" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E57" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E20" t="s">
+    <row r="58" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E58" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E21" t="s">
+    <row r="59" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E59" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="60" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E60" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="61" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E61" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="62" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E62" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E22" t="s">
+    <row r="63" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C63" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="64" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D64" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E65" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E66" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E67" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E68" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E69" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
+    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C71" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C24" t="s">
+    <row r="72" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D72" s="1" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D25" s="1" t="s">
+    <row r="73" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E73" s="4" t="s">
         <v>195</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E26" t="s">
-        <v>196</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Phylogenie : ajout des Coralligene
</commit_message>
<xml_diff>
--- a/other_files/phylogeny.xlsx
+++ b/other_files/phylogeny.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Coraux" sheetId="1" r:id="rId1"/>
-    <sheet name="Mangroves" sheetId="3" r:id="rId2"/>
-    <sheet name="Herbiers" sheetId="2" r:id="rId3"/>
+    <sheet name="Herbiers" sheetId="2" r:id="rId2"/>
+    <sheet name="Mangroves" sheetId="3" r:id="rId3"/>
+    <sheet name="Coralligene" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="342">
   <si>
     <t>Acroporidae</t>
   </si>
@@ -761,6 +762,297 @@
   </si>
   <si>
     <t>Kandelia obovata</t>
+  </si>
+  <si>
+    <t>Felicinia marginata</t>
+  </si>
+  <si>
+    <t>Kallymeniaceae</t>
+  </si>
+  <si>
+    <t>Gigartinales</t>
+  </si>
+  <si>
+    <t>Florideophyceae</t>
+  </si>
+  <si>
+    <t>Alsidium corallinum</t>
+  </si>
+  <si>
+    <t>Rhodomelaceae</t>
+  </si>
+  <si>
+    <t>Ceramiales</t>
+  </si>
+  <si>
+    <t>Arthrocladia villosa</t>
+  </si>
+  <si>
+    <t>Arthrocladiaceae</t>
+  </si>
+  <si>
+    <t>Desmarestiales</t>
+  </si>
+  <si>
+    <t>Phaeophyceae</t>
+  </si>
+  <si>
+    <t>Asperococcus bullosus</t>
+  </si>
+  <si>
+    <t>Chordariaceae</t>
+  </si>
+  <si>
+    <t>Ectocarpales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blastophysa rhizopus </t>
+  </si>
+  <si>
+    <t>Ulvophyceae</t>
+  </si>
+  <si>
+    <t>Boergeseniella fruticulosa</t>
+  </si>
+  <si>
+    <t>Brongniartella byssoides</t>
+  </si>
+  <si>
+    <t>Carpomitra costata</t>
+  </si>
+  <si>
+    <t>Sporochnaceae</t>
+  </si>
+  <si>
+    <t>Sporochnales</t>
+  </si>
+  <si>
+    <t>Chrysymenia ventricosa</t>
+  </si>
+  <si>
+    <t>Rhodymeniaceae</t>
+  </si>
+  <si>
+    <t>Rhodymeniales</t>
+  </si>
+  <si>
+    <t>Cladophora prolifera</t>
+  </si>
+  <si>
+    <t>Cladophoraceae</t>
+  </si>
+  <si>
+    <t>Cladophorales</t>
+  </si>
+  <si>
+    <t>Cutleria chilosa</t>
+  </si>
+  <si>
+    <t>Cutleriaceae</t>
+  </si>
+  <si>
+    <t>Cutleriales</t>
+  </si>
+  <si>
+    <t>Cystoseira foeniculacea</t>
+  </si>
+  <si>
+    <t>Sargassaceae</t>
+  </si>
+  <si>
+    <t>Fucales</t>
+  </si>
+  <si>
+    <t>Cystoseira spinosa</t>
+  </si>
+  <si>
+    <t>Cystoseira usneoides</t>
+  </si>
+  <si>
+    <t>Cystoseira zosteroides</t>
+  </si>
+  <si>
+    <t>Flabellia petiolata</t>
+  </si>
+  <si>
+    <t>Udoteaceae</t>
+  </si>
+  <si>
+    <t>Bryopsidales</t>
+  </si>
+  <si>
+    <t>Gloiocladia repens</t>
+  </si>
+  <si>
+    <t>Faucheaceae</t>
+  </si>
+  <si>
+    <t>Gracilaria corallicola</t>
+  </si>
+  <si>
+    <t>Gracilariaceae</t>
+  </si>
+  <si>
+    <t>Gracilariales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Halarachnion ligulatum </t>
+  </si>
+  <si>
+    <t>Furcellariaceae</t>
+  </si>
+  <si>
+    <t>Halimeda tuna</t>
+  </si>
+  <si>
+    <t>Halimedaceae</t>
+  </si>
+  <si>
+    <t>Halymenia floresii</t>
+  </si>
+  <si>
+    <t>Halymeniaceae</t>
+  </si>
+  <si>
+    <t>Halymeniales</t>
+  </si>
+  <si>
+    <t>Laminaria rodriguezii</t>
+  </si>
+  <si>
+    <t>Laminariaceae</t>
+  </si>
+  <si>
+    <t>Laminariales</t>
+  </si>
+  <si>
+    <t>Lithophyllum stictiforme</t>
+  </si>
+  <si>
+    <t>Lithophyllaceae</t>
+  </si>
+  <si>
+    <t>Corallinales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mesophyllum expansum </t>
+  </si>
+  <si>
+    <t>Hapalidiaceae</t>
+  </si>
+  <si>
+    <t>Hapalidiales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mesophyllum macroblastum </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Palmophyllum crassum </t>
+  </si>
+  <si>
+    <t>Palmophyllaceae</t>
+  </si>
+  <si>
+    <t>Palmophyllales</t>
+  </si>
+  <si>
+    <t>Palmophyllophyceae</t>
+  </si>
+  <si>
+    <t>Peyssonnelia atropurpurea</t>
+  </si>
+  <si>
+    <t>Peyssonneliaceae</t>
+  </si>
+  <si>
+    <t>Peyssonnelia harveyana</t>
+  </si>
+  <si>
+    <t>Peyssonnelia inamoena</t>
+  </si>
+  <si>
+    <t>Peyssonnelia polymorpha</t>
+  </si>
+  <si>
+    <t>Peyssonnelia rubra</t>
+  </si>
+  <si>
+    <t>Peyssonnelia squamaria</t>
+  </si>
+  <si>
+    <t>Phyllariopsis brevipes</t>
+  </si>
+  <si>
+    <t>Phyllariaceae</t>
+  </si>
+  <si>
+    <t>Tilopteridales</t>
+  </si>
+  <si>
+    <t>Phyllophora crispa</t>
+  </si>
+  <si>
+    <t>Phyllophoraceae</t>
+  </si>
+  <si>
+    <t>Polysiphonia elongata</t>
+  </si>
+  <si>
+    <t>Polysiphonia subulifera</t>
+  </si>
+  <si>
+    <t>Sargassum acinarium</t>
+  </si>
+  <si>
+    <t>Sargassum vulgare</t>
+  </si>
+  <si>
+    <t>Scinaia furcellata</t>
+  </si>
+  <si>
+    <t>Scinaiaceae</t>
+  </si>
+  <si>
+    <t>Nemaliales</t>
+  </si>
+  <si>
+    <t>Sphaerococcus coronopifolius</t>
+  </si>
+  <si>
+    <t>Sphaerococcaceae </t>
+  </si>
+  <si>
+    <t>Sphondylothamnion multifidum</t>
+  </si>
+  <si>
+    <t>Ceramiaceae</t>
+  </si>
+  <si>
+    <t>Sporochnus pedunculatus</t>
+  </si>
+  <si>
+    <t>Sporolithon ptychoides</t>
+  </si>
+  <si>
+    <t>Sporolithaceae</t>
+  </si>
+  <si>
+    <t>Sporolithales</t>
+  </si>
+  <si>
+    <t>Zanardinia typus</t>
+  </si>
+  <si>
+    <t>Zonaria tournefortii</t>
+  </si>
+  <si>
+    <t>Dictyotaceae</t>
+  </si>
+  <si>
+    <t>Dictyotales</t>
+  </si>
+  <si>
+    <t>Chaetosiphonaceae</t>
   </si>
 </sst>
 </file>
@@ -1885,9 +2177,116 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>170</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+    <sheetView topLeftCell="A55" workbookViewId="0">
       <selection activeCell="E56" sqref="E56"/>
     </sheetView>
   </sheetViews>
@@ -2289,105 +2688,519 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:D98"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="E93" sqref="E93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B1" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>170</v>
+      <c r="D1" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C4" s="1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D5" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D6" s="1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D7" s="1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D8" s="1" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D9" s="1" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C11" s="1" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D12" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C14" s="1" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D15" s="1" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C16" s="1" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D17" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C18" s="1" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D19" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C20" s="1" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D21" s="1" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D22" s="1" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D23" s="1" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D24" s="1" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D25" s="1" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D26" s="1" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C27" s="1" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D28" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C29" s="1" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D30" s="1" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B31" s="1" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C32" s="1" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D33" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34" s="1" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C35" s="1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D36" s="1" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B37" s="1" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C38" s="1" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D39" s="1" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D40" s="1" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B41" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C42" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D43" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B44" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C45" s="1" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D46" s="1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C47" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D48" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B49" s="1" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C50" s="1" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D51" s="1" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B53" s="1" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C54" s="1" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D55" s="1" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B57" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C58" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D59" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D60" s="1" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B61" s="1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C62" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D63" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B64" s="1" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C65" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D66" s="1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B67" s="1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C68" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D69" s="1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B70" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C71" s="1" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D72" s="1" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D73" s="1" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D74" s="1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D75" s="1" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D76" s="1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D77" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="78" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B78" s="1" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="79" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C79" s="1" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="80" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D80" s="1" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B81" s="1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C82" s="1" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D83" s="1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D84" s="1" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B85" s="1" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C86" s="1" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D87" s="1" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B89" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C90" s="1" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D91" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C92" s="1" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D93" s="1" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C94" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D95" s="1" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B96" s="1" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="97" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C97" s="1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="98" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D98" s="1" t="s">
+        <v>269</v>
       </c>
     </row>
   </sheetData>

</xml_diff>